<commit_message>
APP Nueva Version SUB CARPETAS
</commit_message>
<xml_diff>
--- a/archivos_usuarios/20240823_100703/DIAN.xlsx
+++ b/archivos_usuarios/20240823_100703/DIAN.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcamacho\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcamacho\Desktop\APP PRUEBA\archivos_usuarios\20240823_100703\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613EA25C-1820-48BC-868F-CEB9307C7418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D32C6E7-DA8C-44CC-A7D4-A5A38762DAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>Tipo de documento</t>
   </si>
@@ -164,123 +164,6 @@
   </si>
   <si>
     <t>AMERICAN  LIGHTING  S.A.S</t>
-  </si>
-  <si>
-    <t>8dad5b9441c86262195135aea9f281e81a903a4b00d94599bd0642f5150e6a9d9b3de2099b2c9843fde285fec478dfb2</t>
-  </si>
-  <si>
-    <t>8212</t>
-  </si>
-  <si>
-    <t>FENS</t>
-  </si>
-  <si>
-    <t>15-08-2024 23:27:52</t>
-  </si>
-  <si>
-    <t>52430291</t>
-  </si>
-  <si>
-    <t>NELLY CARMENSA FIGUEROA ANACONA</t>
-  </si>
-  <si>
-    <t>AMERICAN LIGHTING S.A.S.</t>
-  </si>
-  <si>
-    <t>a6897886c2d38efdd5561eb6eaffc9533eecd40112f2730fc6cae0dd9b9f8214d39dba8a2e904c2aa62c227ffc071647</t>
-  </si>
-  <si>
-    <t>312</t>
-  </si>
-  <si>
-    <t>FMS</t>
-  </si>
-  <si>
-    <t>16-08-2024 02:32:26</t>
-  </si>
-  <si>
-    <t>900381637</t>
-  </si>
-  <si>
-    <t>FINANCIAL AND MANAGEMENT SOLUTIONS S.A.S.</t>
-  </si>
-  <si>
-    <t>c83ff3a5189b37304cdd0ed9e4a8c4ff00aa156e7e27cb714bd16d868f9c1092c735ec1a50a1d93f710cda83fd1f0b77</t>
-  </si>
-  <si>
-    <t>43721</t>
-  </si>
-  <si>
-    <t>FE</t>
-  </si>
-  <si>
-    <t>16-08-2024 01:38:00</t>
-  </si>
-  <si>
-    <t>901237887</t>
-  </si>
-  <si>
-    <t>EDS EL POBLADO PRAGOM SAS ZOMAC</t>
-  </si>
-  <si>
-    <t>d9dc2587bcdc1005288e20263ed0f8696232cf04557d1acbdf6248cfa11719e18efd6843d904187e856ae97f0717605a</t>
-  </si>
-  <si>
-    <t>50704</t>
-  </si>
-  <si>
-    <t>FE01</t>
-  </si>
-  <si>
-    <t>15-08-2024 22:02:09</t>
-  </si>
-  <si>
-    <t>901260162</t>
-  </si>
-  <si>
-    <t>ALMACENES UNIVERSAL S.A.S.</t>
-  </si>
-  <si>
-    <t>799b12b73c4de1f63f81ede3739c4f1e9321bfcc58aa08733c2dd3b168bfb01a6018a475215143045cac79703476816f</t>
-  </si>
-  <si>
-    <t>162268</t>
-  </si>
-  <si>
-    <t>CTGN</t>
-  </si>
-  <si>
-    <t>14-08-2024</t>
-  </si>
-  <si>
-    <t>14-08-2024 20:35:34</t>
-  </si>
-  <si>
-    <t>890404087</t>
-  </si>
-  <si>
-    <t>AGENCIA DE ADUANAS IMEX S.A.S. NIVEL 1</t>
-  </si>
-  <si>
-    <t>American Lighting S.A.S.</t>
-  </si>
-  <si>
-    <t>4b5c1f10d86452004008ee7bcb690cd6e3806b6365ba9c4ea10ccc74fb2054e624eb7e6c6a9a866aa3a21d1adc667dd4</t>
-  </si>
-  <si>
-    <t>37645</t>
-  </si>
-  <si>
-    <t>KF01</t>
-  </si>
-  <si>
-    <t>14-08-2024 19:47:58</t>
-  </si>
-  <si>
-    <t>900491889</t>
-  </si>
-  <si>
-    <t>MASSER S A S</t>
   </si>
 </sst>
 </file>
@@ -648,7 +531,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -921,306 +804,6 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K6" s="1">
-        <v>27408</v>
-      </c>
-      <c r="L6" s="1">
-        <v>0</v>
-      </c>
-      <c r="M6" s="1">
-        <v>0</v>
-      </c>
-      <c r="N6" s="1">
-        <v>171662</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K7" s="1">
-        <v>603801</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
-      <c r="N7" s="1">
-        <v>3781701</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0</v>
-      </c>
-      <c r="L8" s="1">
-        <v>0</v>
-      </c>
-      <c r="M8" s="1">
-        <v>0</v>
-      </c>
-      <c r="N8" s="1">
-        <v>150000</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" s="1">
-        <v>5588.24</v>
-      </c>
-      <c r="L9" s="1">
-        <v>0</v>
-      </c>
-      <c r="M9" s="1">
-        <v>0</v>
-      </c>
-      <c r="N9" s="1">
-        <v>35000</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K10" s="1">
-        <v>0</v>
-      </c>
-      <c r="L10" s="1">
-        <v>0</v>
-      </c>
-      <c r="M10" s="1">
-        <v>0</v>
-      </c>
-      <c r="N10" s="1">
-        <v>1305200</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="1">
-        <v>0</v>
-      </c>
-      <c r="L11" s="1">
-        <v>0</v>
-      </c>
-      <c r="M11" s="1">
-        <v>0</v>
-      </c>
-      <c r="N11" s="1">
-        <v>136723</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>